<commit_message>
Midterm Grades for IT 1A, CS 3B, CS 3C
</commit_message>
<xml_diff>
--- a/DCIT 55 - IT 3G/LEC AND LAB.xlsx
+++ b/DCIT 55 - IT 3G/LEC AND LAB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRATION" sheetId="1" r:id="rId1"/>
@@ -2375,9 +2375,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2444,6 +2441,9 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -2496,6 +2496,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -2503,9 +2506,6 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3426,8 +3426,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5337,9 +5337,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:CU70"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="CN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CO10" sqref="CO10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="BL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BT18" sqref="BT18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5558,130 +5558,130 @@
     </row>
     <row r="4" spans="1:99" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="176" t="s">
+      <c r="B5" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="177" t="s">
+      <c r="D5" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
-      <c r="G5" s="178"/>
-      <c r="H5" s="178"/>
-      <c r="I5" s="178"/>
-      <c r="J5" s="178"/>
-      <c r="K5" s="178"/>
-      <c r="L5" s="178"/>
-      <c r="M5" s="178"/>
-      <c r="N5" s="178"/>
-      <c r="O5" s="178"/>
-      <c r="P5" s="178"/>
-      <c r="Q5" s="178"/>
-      <c r="R5" s="178"/>
-      <c r="S5" s="178"/>
-      <c r="T5" s="178"/>
-      <c r="U5" s="178"/>
-      <c r="V5" s="178"/>
-      <c r="W5" s="178"/>
-      <c r="X5" s="178"/>
-      <c r="Y5" s="178"/>
-      <c r="Z5" s="178"/>
-      <c r="AA5" s="178"/>
-      <c r="AB5" s="178"/>
-      <c r="AC5" s="178"/>
-      <c r="AD5" s="178"/>
-      <c r="AE5" s="178"/>
-      <c r="AF5" s="178"/>
-      <c r="AG5" s="178"/>
-      <c r="AH5" s="178"/>
-      <c r="AI5" s="178"/>
-      <c r="AJ5" s="178"/>
-      <c r="AK5" s="178"/>
-      <c r="AL5" s="178"/>
-      <c r="AM5" s="178"/>
-      <c r="AN5" s="178"/>
-      <c r="AO5" s="178"/>
-      <c r="AP5" s="178"/>
-      <c r="AQ5" s="178"/>
-      <c r="AR5" s="178"/>
-      <c r="AS5" s="178"/>
-      <c r="AT5" s="178"/>
-      <c r="AU5" s="178"/>
-      <c r="AV5" s="178"/>
-      <c r="AW5" s="178"/>
-      <c r="AX5" s="178"/>
-      <c r="AY5" s="178"/>
-      <c r="AZ5" s="178"/>
-      <c r="BA5" s="178"/>
-      <c r="BB5" s="178"/>
-      <c r="BC5" s="178"/>
-      <c r="BD5" s="179"/>
-      <c r="BE5" s="180" t="s">
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="177"/>
+      <c r="Q5" s="177"/>
+      <c r="R5" s="177"/>
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="177"/>
+      <c r="Y5" s="177"/>
+      <c r="Z5" s="177"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="177"/>
+      <c r="AC5" s="177"/>
+      <c r="AD5" s="177"/>
+      <c r="AE5" s="177"/>
+      <c r="AF5" s="177"/>
+      <c r="AG5" s="177"/>
+      <c r="AH5" s="177"/>
+      <c r="AI5" s="177"/>
+      <c r="AJ5" s="177"/>
+      <c r="AK5" s="177"/>
+      <c r="AL5" s="177"/>
+      <c r="AM5" s="177"/>
+      <c r="AN5" s="177"/>
+      <c r="AO5" s="177"/>
+      <c r="AP5" s="177"/>
+      <c r="AQ5" s="177"/>
+      <c r="AR5" s="177"/>
+      <c r="AS5" s="177"/>
+      <c r="AT5" s="177"/>
+      <c r="AU5" s="177"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="AX5" s="177"/>
+      <c r="AY5" s="177"/>
+      <c r="AZ5" s="177"/>
+      <c r="BA5" s="177"/>
+      <c r="BB5" s="177"/>
+      <c r="BC5" s="177"/>
+      <c r="BD5" s="178"/>
+      <c r="BE5" s="179" t="s">
         <v>34</v>
       </c>
-      <c r="BF5" s="181"/>
-      <c r="BG5" s="181"/>
-      <c r="BH5" s="181"/>
-      <c r="BI5" s="181"/>
-      <c r="BJ5" s="181"/>
-      <c r="BK5" s="181"/>
-      <c r="BL5" s="181"/>
-      <c r="BM5" s="181"/>
-      <c r="BN5" s="181"/>
-      <c r="BO5" s="181"/>
-      <c r="BP5" s="181"/>
-      <c r="BQ5" s="181"/>
-      <c r="BR5" s="181"/>
-      <c r="BS5" s="181"/>
-      <c r="BT5" s="181"/>
-      <c r="BU5" s="181"/>
-      <c r="BV5" s="181"/>
-      <c r="BW5" s="181"/>
-      <c r="BX5" s="181"/>
-      <c r="BY5" s="181"/>
-      <c r="BZ5" s="181"/>
-      <c r="CA5" s="181"/>
-      <c r="CB5" s="181"/>
-      <c r="CC5" s="181"/>
-      <c r="CD5" s="181"/>
-      <c r="CE5" s="181"/>
-      <c r="CF5" s="181"/>
-      <c r="CG5" s="181"/>
-      <c r="CH5" s="181"/>
-      <c r="CI5" s="181"/>
-      <c r="CJ5" s="181"/>
-      <c r="CK5" s="181"/>
-      <c r="CL5" s="181"/>
-      <c r="CM5" s="181"/>
-      <c r="CN5" s="181"/>
-      <c r="CO5" s="181"/>
-      <c r="CP5" s="181"/>
-      <c r="CQ5" s="181"/>
-      <c r="CR5" s="182"/>
-      <c r="CS5" s="187" t="s">
+      <c r="BF5" s="180"/>
+      <c r="BG5" s="180"/>
+      <c r="BH5" s="180"/>
+      <c r="BI5" s="180"/>
+      <c r="BJ5" s="180"/>
+      <c r="BK5" s="180"/>
+      <c r="BL5" s="180"/>
+      <c r="BM5" s="180"/>
+      <c r="BN5" s="180"/>
+      <c r="BO5" s="180"/>
+      <c r="BP5" s="180"/>
+      <c r="BQ5" s="180"/>
+      <c r="BR5" s="180"/>
+      <c r="BS5" s="180"/>
+      <c r="BT5" s="180"/>
+      <c r="BU5" s="180"/>
+      <c r="BV5" s="180"/>
+      <c r="BW5" s="180"/>
+      <c r="BX5" s="180"/>
+      <c r="BY5" s="180"/>
+      <c r="BZ5" s="180"/>
+      <c r="CA5" s="180"/>
+      <c r="CB5" s="180"/>
+      <c r="CC5" s="180"/>
+      <c r="CD5" s="180"/>
+      <c r="CE5" s="180"/>
+      <c r="CF5" s="180"/>
+      <c r="CG5" s="180"/>
+      <c r="CH5" s="180"/>
+      <c r="CI5" s="180"/>
+      <c r="CJ5" s="180"/>
+      <c r="CK5" s="180"/>
+      <c r="CL5" s="180"/>
+      <c r="CM5" s="180"/>
+      <c r="CN5" s="180"/>
+      <c r="CO5" s="180"/>
+      <c r="CP5" s="180"/>
+      <c r="CQ5" s="180"/>
+      <c r="CR5" s="181"/>
+      <c r="CS5" s="186" t="s">
         <v>35</v>
       </c>
-      <c r="CT5" s="188"/>
-      <c r="CU5" s="189"/>
+      <c r="CT5" s="187"/>
+      <c r="CU5" s="188"/>
     </row>
     <row r="6" spans="1:99" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="174"/>
-      <c r="B6" s="176"/>
-      <c r="C6" s="176"/>
-      <c r="D6" s="205" t="s">
+      <c r="A6" s="173"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="175"/>
+      <c r="D6" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="206"/>
-      <c r="F6" s="206"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="206"/>
-      <c r="I6" s="206"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="207"/>
+      <c r="G6" s="207"/>
+      <c r="H6" s="207"/>
+      <c r="I6" s="207"/>
       <c r="J6" s="190" t="s">
         <v>140</v>
       </c>
@@ -5781,14 +5781,14 @@
       <c r="CN6" s="197"/>
       <c r="CO6" s="197"/>
       <c r="CP6" s="197"/>
-      <c r="CQ6" s="171" t="s">
+      <c r="CQ6" s="189" t="s">
         <v>40</v>
       </c>
-      <c r="CR6" s="171"/>
-      <c r="CS6" s="172" t="s">
+      <c r="CR6" s="189"/>
+      <c r="CS6" s="171" t="s">
         <v>41</v>
       </c>
-      <c r="CT6" s="172" t="s">
+      <c r="CT6" s="171" t="s">
         <v>42</v>
       </c>
       <c r="CU6" s="191" t="s">
@@ -5796,9 +5796,9 @@
       </c>
     </row>
     <row r="7" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A7" s="174"/>
-      <c r="B7" s="176"/>
-      <c r="C7" s="176"/>
+      <c r="A7" s="173"/>
+      <c r="B7" s="175"/>
+      <c r="C7" s="175"/>
       <c r="E7" s="124"/>
       <c r="F7" s="123">
         <v>0.3</v>
@@ -5807,244 +5807,244 @@
       <c r="I7" s="124">
         <v>0.3</v>
       </c>
-      <c r="J7" s="185"/>
-      <c r="K7" s="185"/>
-      <c r="L7" s="185"/>
-      <c r="M7" s="185"/>
-      <c r="N7" s="185"/>
-      <c r="O7" s="185"/>
-      <c r="P7" s="185"/>
-      <c r="Q7" s="185"/>
-      <c r="R7" s="185"/>
-      <c r="S7" s="185"/>
-      <c r="T7" s="186">
+      <c r="J7" s="184"/>
+      <c r="K7" s="184"/>
+      <c r="L7" s="184"/>
+      <c r="M7" s="184"/>
+      <c r="N7" s="184"/>
+      <c r="O7" s="184"/>
+      <c r="P7" s="184"/>
+      <c r="Q7" s="184"/>
+      <c r="R7" s="184"/>
+      <c r="S7" s="184"/>
+      <c r="T7" s="185">
         <f>COUNT(J9,L9,N9,P9,R9,T9)</f>
         <v>0</v>
       </c>
-      <c r="U7" s="186"/>
-      <c r="V7" s="185"/>
-      <c r="W7" s="185"/>
-      <c r="X7" s="185"/>
-      <c r="Y7" s="185"/>
-      <c r="Z7" s="185"/>
-      <c r="AA7" s="185"/>
-      <c r="AB7" s="185"/>
-      <c r="AC7" s="185"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="185"/>
-      <c r="AF7" s="185"/>
-      <c r="AG7" s="185"/>
-      <c r="AH7" s="185"/>
-      <c r="AI7" s="185"/>
-      <c r="AJ7" s="185"/>
-      <c r="AK7" s="185"/>
-      <c r="AL7" s="185"/>
-      <c r="AM7" s="185"/>
+      <c r="U7" s="185"/>
+      <c r="V7" s="184"/>
+      <c r="W7" s="184"/>
+      <c r="X7" s="184"/>
+      <c r="Y7" s="184"/>
+      <c r="Z7" s="184"/>
+      <c r="AA7" s="184"/>
+      <c r="AB7" s="184"/>
+      <c r="AC7" s="184"/>
+      <c r="AD7" s="184"/>
+      <c r="AE7" s="184"/>
+      <c r="AF7" s="184"/>
+      <c r="AG7" s="184"/>
+      <c r="AH7" s="184"/>
+      <c r="AI7" s="184"/>
+      <c r="AJ7" s="184"/>
+      <c r="AK7" s="184"/>
+      <c r="AL7" s="184"/>
+      <c r="AM7" s="184"/>
       <c r="AN7" s="97">
         <v>0.2</v>
       </c>
-      <c r="AO7" s="185"/>
-      <c r="AP7" s="185"/>
-      <c r="AQ7" s="185"/>
-      <c r="AR7" s="185"/>
-      <c r="AS7" s="186">
+      <c r="AO7" s="184"/>
+      <c r="AP7" s="184"/>
+      <c r="AQ7" s="184"/>
+      <c r="AR7" s="184"/>
+      <c r="AS7" s="185">
         <f>COUNT(AO9,AQ9,AS9)</f>
         <v>0</v>
       </c>
-      <c r="AT7" s="186"/>
+      <c r="AT7" s="185"/>
       <c r="AU7" s="21">
         <v>0.1</v>
       </c>
-      <c r="AV7" s="185"/>
-      <c r="AW7" s="185"/>
-      <c r="AX7" s="185"/>
-      <c r="AY7" s="185"/>
-      <c r="AZ7" s="186">
+      <c r="AV7" s="184"/>
+      <c r="AW7" s="184"/>
+      <c r="AX7" s="184"/>
+      <c r="AY7" s="184"/>
+      <c r="AZ7" s="185">
         <f>COUNT(AV9,AX9,AZ9)</f>
         <v>0</v>
       </c>
-      <c r="BA7" s="186"/>
+      <c r="BA7" s="185"/>
       <c r="BB7" s="22">
         <v>0.1</v>
       </c>
       <c r="BC7" s="194"/>
       <c r="BD7" s="195"/>
-      <c r="BE7" s="185" t="s">
+      <c r="BE7" s="184" t="s">
         <v>232</v>
       </c>
-      <c r="BF7" s="185"/>
-      <c r="BG7" s="185" t="s">
+      <c r="BF7" s="184"/>
+      <c r="BG7" s="184" t="s">
         <v>232</v>
       </c>
-      <c r="BH7" s="185"/>
-      <c r="BI7" s="186">
+      <c r="BH7" s="184"/>
+      <c r="BI7" s="185">
         <f>COUNT(BE9,BG9,BI9)</f>
         <v>2</v>
       </c>
-      <c r="BJ7" s="186"/>
+      <c r="BJ7" s="185"/>
       <c r="BK7" s="105">
         <v>0.5</v>
       </c>
-      <c r="BL7" s="185">
+      <c r="BL7" s="184">
         <v>42980</v>
       </c>
-      <c r="BM7" s="185"/>
-      <c r="BN7" s="185">
+      <c r="BM7" s="184"/>
+      <c r="BN7" s="184">
         <v>42980</v>
       </c>
-      <c r="BO7" s="185"/>
-      <c r="BP7" s="185">
+      <c r="BO7" s="184"/>
+      <c r="BP7" s="184">
         <v>42980</v>
       </c>
-      <c r="BQ7" s="185"/>
-      <c r="BR7" s="185">
+      <c r="BQ7" s="184"/>
+      <c r="BR7" s="184">
         <v>42987</v>
       </c>
-      <c r="BS7" s="185"/>
-      <c r="BT7" s="185"/>
-      <c r="BU7" s="185"/>
-      <c r="BV7" s="185"/>
-      <c r="BW7" s="185"/>
-      <c r="BX7" s="185"/>
-      <c r="BY7" s="185"/>
-      <c r="BZ7" s="185"/>
-      <c r="CA7" s="185"/>
-      <c r="CB7" s="185"/>
-      <c r="CC7" s="185"/>
-      <c r="CD7" s="185"/>
-      <c r="CE7" s="185"/>
-      <c r="CF7" s="185"/>
-      <c r="CG7" s="185"/>
-      <c r="CH7" s="185"/>
-      <c r="CI7" s="185"/>
-      <c r="CJ7" s="185"/>
-      <c r="CK7" s="185"/>
-      <c r="CL7" s="185"/>
-      <c r="CM7" s="185"/>
-      <c r="CN7" s="186">
+      <c r="BS7" s="184"/>
+      <c r="BT7" s="184"/>
+      <c r="BU7" s="184"/>
+      <c r="BV7" s="184"/>
+      <c r="BW7" s="184"/>
+      <c r="BX7" s="184"/>
+      <c r="BY7" s="184"/>
+      <c r="BZ7" s="184"/>
+      <c r="CA7" s="184"/>
+      <c r="CB7" s="184"/>
+      <c r="CC7" s="184"/>
+      <c r="CD7" s="184"/>
+      <c r="CE7" s="184"/>
+      <c r="CF7" s="184"/>
+      <c r="CG7" s="184"/>
+      <c r="CH7" s="184"/>
+      <c r="CI7" s="184"/>
+      <c r="CJ7" s="184"/>
+      <c r="CK7" s="184"/>
+      <c r="CL7" s="184"/>
+      <c r="CM7" s="184"/>
+      <c r="CN7" s="185">
         <f>COUNT(CN9,CL9,CJ9,CH9,CF9,CD9,CB9,BZ9,BX9,BV9,BT9,BR9,BP9,BN9,BL9)</f>
         <v>5</v>
       </c>
-      <c r="CO7" s="186"/>
+      <c r="CO7" s="185"/>
       <c r="CP7" s="106">
         <v>0.5</v>
       </c>
-      <c r="CQ7" s="171"/>
-      <c r="CR7" s="171"/>
-      <c r="CS7" s="172"/>
-      <c r="CT7" s="172"/>
+      <c r="CQ7" s="189"/>
+      <c r="CR7" s="189"/>
+      <c r="CS7" s="171"/>
+      <c r="CT7" s="171"/>
       <c r="CU7" s="192"/>
     </row>
     <row r="8" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A8" s="174"/>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-      <c r="D8" s="183" t="s">
+      <c r="A8" s="173"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="175"/>
+      <c r="D8" s="182" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="183" t="s">
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182" t="s">
         <v>158</v>
       </c>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="184" t="s">
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
+      <c r="J8" s="183" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="184"/>
-      <c r="L8" s="184" t="s">
+      <c r="K8" s="183"/>
+      <c r="L8" s="183" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="184"/>
-      <c r="N8" s="184" t="s">
+      <c r="M8" s="183"/>
+      <c r="N8" s="183" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="184"/>
-      <c r="P8" s="184" t="s">
+      <c r="O8" s="183"/>
+      <c r="P8" s="183" t="s">
         <v>51</v>
       </c>
-      <c r="Q8" s="184"/>
-      <c r="R8" s="184" t="s">
+      <c r="Q8" s="183"/>
+      <c r="R8" s="183" t="s">
         <v>52</v>
       </c>
-      <c r="S8" s="184"/>
-      <c r="T8" s="184" t="s">
+      <c r="S8" s="183"/>
+      <c r="T8" s="183" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="184"/>
-      <c r="V8" s="184" t="s">
+      <c r="U8" s="183"/>
+      <c r="V8" s="183" t="s">
         <v>54</v>
       </c>
-      <c r="W8" s="184"/>
-      <c r="X8" s="184" t="s">
+      <c r="W8" s="183"/>
+      <c r="X8" s="183" t="s">
         <v>55</v>
       </c>
-      <c r="Y8" s="184"/>
-      <c r="Z8" s="184" t="s">
+      <c r="Y8" s="183"/>
+      <c r="Z8" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="184"/>
-      <c r="AB8" s="184" t="s">
+      <c r="AA8" s="183"/>
+      <c r="AB8" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="184"/>
-      <c r="AD8" s="184" t="s">
+      <c r="AC8" s="183"/>
+      <c r="AD8" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="AE8" s="184"/>
-      <c r="AF8" s="184" t="s">
+      <c r="AE8" s="183"/>
+      <c r="AF8" s="183" t="s">
         <v>59</v>
       </c>
-      <c r="AG8" s="184"/>
-      <c r="AH8" s="184" t="s">
+      <c r="AG8" s="183"/>
+      <c r="AH8" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="AI8" s="184"/>
-      <c r="AJ8" s="184" t="s">
+      <c r="AI8" s="183"/>
+      <c r="AJ8" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="AK8" s="184"/>
-      <c r="AL8" s="184" t="s">
+      <c r="AK8" s="183"/>
+      <c r="AL8" s="183" t="s">
         <v>62</v>
       </c>
-      <c r="AM8" s="184"/>
+      <c r="AM8" s="183"/>
       <c r="AN8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AO8" s="184" t="s">
+      <c r="AO8" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="AP8" s="184"/>
-      <c r="AQ8" s="184" t="s">
+      <c r="AP8" s="183"/>
+      <c r="AQ8" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AR8" s="184"/>
-      <c r="AS8" s="184" t="s">
+      <c r="AR8" s="183"/>
+      <c r="AS8" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="AT8" s="184"/>
+      <c r="AT8" s="183"/>
       <c r="AU8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AV8" s="184" t="s">
+      <c r="AV8" s="183" t="s">
         <v>68</v>
       </c>
-      <c r="AW8" s="184"/>
-      <c r="AX8" s="184" t="s">
+      <c r="AW8" s="183"/>
+      <c r="AX8" s="183" t="s">
         <v>69</v>
       </c>
-      <c r="AY8" s="184"/>
-      <c r="AZ8" s="184" t="s">
+      <c r="AY8" s="183"/>
+      <c r="AZ8" s="183" t="s">
         <v>70</v>
       </c>
-      <c r="BA8" s="184"/>
+      <c r="BA8" s="183"/>
       <c r="BB8" s="25" t="s">
         <v>71</v>
       </c>
       <c r="BC8" s="194"/>
       <c r="BD8" s="195"/>
-      <c r="BE8" s="207" t="s">
+      <c r="BE8" s="205" t="s">
         <v>44</v>
       </c>
       <c r="BF8" s="202"/>
@@ -6122,16 +6122,16 @@
       <c r="CP8" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="CQ8" s="171"/>
-      <c r="CR8" s="171"/>
-      <c r="CS8" s="172"/>
-      <c r="CT8" s="172"/>
+      <c r="CQ8" s="189"/>
+      <c r="CR8" s="189"/>
+      <c r="CS8" s="171"/>
+      <c r="CT8" s="171"/>
       <c r="CU8" s="192"/>
     </row>
     <row r="9" spans="1:99" ht="15.75" thickBot="1">
-      <c r="A9" s="175"/>
-      <c r="B9" s="176"/>
-      <c r="C9" s="176"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="175"/>
       <c r="D9" s="27"/>
       <c r="E9" s="91"/>
       <c r="F9" s="28" t="s">
@@ -6297,8 +6297,8 @@
       <c r="CR9" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="CS9" s="172"/>
-      <c r="CT9" s="172"/>
+      <c r="CS9" s="171"/>
+      <c r="CT9" s="171"/>
       <c r="CU9" s="193"/>
     </row>
     <row r="10" spans="1:99">
@@ -10078,11 +10078,11 @@
         <v>100</v>
       </c>
       <c r="BT24" s="108">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BU24" s="92">
         <f t="shared" si="27"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="BV24" s="107"/>
       <c r="BW24" s="92" t="str">
@@ -10136,19 +10136,19 @@
       </c>
       <c r="CP24" s="103">
         <f t="shared" si="38"/>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="CQ24" s="99">
         <f t="shared" si="39"/>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="CR24" s="99">
         <f t="shared" si="40"/>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="CS24" s="104">
         <f t="shared" si="45"/>
-        <v>28.5</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="CT24" s="104">
         <f>IFERROR(VLOOKUP(CS24,REGISTRATION!$P$22:$Q$32,2),"")</f>
@@ -21600,6 +21600,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="98">
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="AV8:AW8"/>
+    <mergeCell ref="AX8:AY8"/>
     <mergeCell ref="A2:CU3"/>
     <mergeCell ref="CB8:CC8"/>
     <mergeCell ref="CD8:CE8"/>
@@ -21613,14 +21617,6 @@
     <mergeCell ref="BV8:BW8"/>
     <mergeCell ref="BX8:BY8"/>
     <mergeCell ref="BZ8:CA8"/>
-    <mergeCell ref="AZ8:BA8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="AD8:AE8"/>
-    <mergeCell ref="AF8:AG8"/>
-    <mergeCell ref="AH8:AI8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="AV8:AW8"/>
-    <mergeCell ref="AX8:AY8"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="X8:Y8"/>
     <mergeCell ref="Z8:AA8"/>
@@ -21635,14 +21631,8 @@
     <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="J6:AN6"/>
     <mergeCell ref="V7:W7"/>
-    <mergeCell ref="CN8:CO8"/>
-    <mergeCell ref="BI7:BJ7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="AL7:AM7"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AF8:AG8"/>
+    <mergeCell ref="AH8:AI8"/>
     <mergeCell ref="BI8:BJ8"/>
     <mergeCell ref="BL8:BM8"/>
     <mergeCell ref="BN8:BO8"/>
@@ -21651,6 +21641,15 @@
     <mergeCell ref="AQ8:AR8"/>
     <mergeCell ref="AS8:AT8"/>
     <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="AZ8:BA8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI7:BJ7"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="AL7:AM7"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS7:AT7"/>
     <mergeCell ref="AO6:AU6"/>
     <mergeCell ref="AV6:BB6"/>
     <mergeCell ref="CU6:CU9"/>
@@ -21667,7 +21666,6 @@
     <mergeCell ref="AF7:AG7"/>
     <mergeCell ref="CT6:CT9"/>
     <mergeCell ref="BE7:BF7"/>
-    <mergeCell ref="CH7:CI7"/>
     <mergeCell ref="CS5:CU5"/>
     <mergeCell ref="BL7:BM7"/>
     <mergeCell ref="BN7:BO7"/>
@@ -21683,6 +21681,7 @@
     <mergeCell ref="CJ7:CK7"/>
     <mergeCell ref="CD7:CE7"/>
     <mergeCell ref="CQ6:CR8"/>
+    <mergeCell ref="CN8:CO8"/>
     <mergeCell ref="CS6:CS9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B5:B9"/>
@@ -21698,6 +21697,7 @@
     <mergeCell ref="AZ7:BA7"/>
     <mergeCell ref="BG7:BH7"/>
     <mergeCell ref="CF7:CG7"/>
+    <mergeCell ref="CH7:CI7"/>
   </mergeCells>
   <conditionalFormatting sqref="CU10:CU70">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -22843,19 +22843,19 @@
       </c>
       <c r="K22" s="52">
         <f>'RAW GRADES'!CP24</f>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="L22" s="52">
         <f>'RAW GRADES'!CQ24</f>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="M22" s="54">
         <f>'RAW GRADES'!CR24</f>
-        <v>47.5</v>
+        <v>48</v>
       </c>
       <c r="N22" s="58">
         <f>'RAW GRADES'!CS24</f>
-        <v>28.5</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="O22" s="56">
         <f>'RAW GRADES'!CT24</f>
@@ -27665,7 +27665,7 @@
       <c r="D87" s="60"/>
       <c r="E87" s="245">
         <f ca="1">NOW()</f>
-        <v>43003.651956712965</v>
+        <v>43019.446550231478</v>
       </c>
       <c r="F87" s="245"/>
     </row>

</xml_diff>